<commit_message>
added orders to db specification
</commit_message>
<xml_diff>
--- a/doc/DB_TradingService.xlsx
+++ b/doc/DB_TradingService.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\r.beck\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\git\bic4-sam\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Methoden" sheetId="3" r:id="rId1"/>
     <sheet name="User" sheetId="1" r:id="rId2"/>
     <sheet name="Depot" sheetId="2" r:id="rId3"/>
+    <sheet name="Order" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>User-ID</t>
   </si>
@@ -86,6 +87,12 @@
   </si>
   <si>
     <t>getDepots(int User-ID, String CompanyName)</t>
+  </si>
+  <si>
+    <t>State (STRING)</t>
+  </si>
+  <si>
+    <t>Type (STRING)</t>
   </si>
 </sst>
 </file>
@@ -598,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -658,7 +665,7 @@
   <dimension ref="B1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="B2:F2"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -727,7 +734,7 @@
   <dimension ref="B1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F6" sqref="B2:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -789,4 +796,58 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="9"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>